<commit_message>
FIX: Fixed a bug in the EXCEL export process
</commit_message>
<xml_diff>
--- a/resources/io/github/erde/generate/excel/template.xlsx
+++ b/resources/io/github/erde/generate/excel/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="3" r:id="rId1"/>
@@ -13,8 +13,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">テーブル一覧!$A$4:$D$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">テーブル定義!$A$7:$L$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">テーブル定義!$A$1:$L$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">テーブル定義!$A$7:$M$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">テーブル定義!$A$1:$M$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">表紙!$A$1:$N$37</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>PK</t>
   </si>
@@ -244,10 +244,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>${column.unique}</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>NOT NULL</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -348,6 +344,18 @@
   </si>
   <si>
     <t>$[HYPERLINK("#${table.physicalTableName}!A1", "${table.logicalTableName}")]</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>${column.unique}</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>オートインクリメント</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>${column.autoIncrement}</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -597,7 +605,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -653,6 +661,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -682,9 +696,6 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -995,25 +1006,25 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="6" spans="1:14" s="18" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
+    <row r="6" spans="1:14" s="18" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1031,47 +1042,47 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" customWidth="1"/>
-    <col min="2" max="3" width="35.6328125" customWidth="1"/>
-    <col min="4" max="4" width="50.6328125" customWidth="1"/>
+    <col min="1" max="1" width="5.625" customWidth="1"/>
+    <col min="2" max="3" width="35.625" customWidth="1"/>
+    <col min="4" max="4" width="50.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="C4" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>26</v>
-      </c>
       <c r="D4" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1084,22 +1095,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="5.6328125" customWidth="1"/>
-    <col min="4" max="5" width="20.6328125" customWidth="1"/>
-    <col min="6" max="6" width="12.6328125" customWidth="1"/>
-    <col min="7" max="9" width="8.6328125" customWidth="1"/>
-    <col min="10" max="11" width="20.6328125" customWidth="1"/>
-    <col min="12" max="12" width="40.6328125" customWidth="1"/>
+    <col min="1" max="3" width="5.625" customWidth="1"/>
+    <col min="4" max="5" width="20.625" customWidth="1"/>
+    <col min="6" max="6" width="12.625" customWidth="1"/>
+    <col min="7" max="10" width="10.625" customWidth="1"/>
+    <col min="11" max="12" width="20.625" customWidth="1"/>
+    <col min="13" max="13" width="40.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="str">
+    <row r="1" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="str">
         <f>HYPERLINK("#テーブル一覧!A1", "テーブル定義")</f>
         <v>テーブル定義</v>
       </c>
@@ -1114,64 +1125,68 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="19"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="19"/>
     </row>
-    <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="26"/>
+      <c r="D3" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="28"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="16"/>
-      <c r="D4" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="29"/>
+      <c r="D4" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="31"/>
     </row>
-    <row r="5" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="32"/>
+      <c r="D5" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="34"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -1184,51 +1199,55 @@
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="20" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A7" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="L7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="M7" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>35</v>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A8" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>8</v>
@@ -1242,30 +1261,33 @@
       <c r="F8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="24" t="s">
         <v>17</v>
       </c>
       <c r="H8" s="22" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="M8" s="17" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D3:L3"/>
-    <mergeCell ref="D4:L4"/>
-    <mergeCell ref="D5:L5"/>
+    <mergeCell ref="D3:M3"/>
+    <mergeCell ref="D4:M4"/>
+    <mergeCell ref="D5:M5"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>